<commit_message>
Updated correct mae results
</commit_message>
<xml_diff>
--- a/MTQE_results.xlsx
+++ b/MTQE_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dockreg/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dockreg/Shared_task_wmt_2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2435408-310F-0B4C-9B8E-AE35224718D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC600488-43F4-664D-83A0-6842645E99D7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{4B31ACE1-BB33-DE4A-A709-415266748029}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{4B31ACE1-BB33-DE4A-A709-415266748029}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>Pearson</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Top result</t>
+  </si>
+  <si>
+    <t>MAE_redo_final</t>
   </si>
 </sst>
 </file>
@@ -298,7 +301,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="98">
+  <dxfs count="26">
     <dxf>
       <border>
         <left style="thin">
@@ -464,6 +467,22 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -490,22 +509,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <color rgb="FF006100"/>
       </font>
@@ -530,750 +533,6 @@
           <color rgb="FF9C0006"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1685,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBA68734-43C1-B244-AD5F-43DCC3FC98C8}">
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:F1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2512,211 +1771,245 @@
         <v>0.41589999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="3" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49">
+        <v>0.84950000000000003</v>
+      </c>
+      <c r="D49">
+        <v>0.80779999999999996</v>
+      </c>
+      <c r="E49">
+        <v>0.37409999999999999</v>
+      </c>
+      <c r="F49">
+        <v>0.50539999999999996</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B51" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C50" s="4">
+      <c r="C51" s="4">
         <v>0.5514</v>
       </c>
-      <c r="D50" s="4">
+      <c r="D51" s="4">
         <v>0.54890000000000005</v>
       </c>
-      <c r="E50" s="4">
+      <c r="E51" s="4">
         <v>0.78039999999999998</v>
       </c>
-      <c r="F50" s="4">
+      <c r="F51" s="4">
         <v>0.95109999999999995</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B51" t="s">
-        <v>28</v>
-      </c>
-      <c r="C51" s="2">
-        <v>0.76690000000000003</v>
-      </c>
-      <c r="D51">
-        <v>0.79339999999999999</v>
-      </c>
-      <c r="E51">
-        <v>0.72030000000000005</v>
-      </c>
-      <c r="F51">
-        <v>0.83760000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52">
-        <v>0.45190000000000002</v>
+        <v>28</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.76690000000000003</v>
       </c>
       <c r="D52">
-        <v>0.4672</v>
+        <v>0.79339999999999999</v>
       </c>
       <c r="E52">
-        <v>0.99729999999999996</v>
+        <v>0.72030000000000005</v>
       </c>
       <c r="F52">
-        <v>1.1705000000000001</v>
+        <v>0.83760000000000001</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C53">
-        <v>0.5696</v>
+        <v>0.45190000000000002</v>
       </c>
       <c r="D53">
-        <v>0.53900000000000003</v>
+        <v>0.4672</v>
       </c>
       <c r="E53">
-        <v>0.80110000000000003</v>
+        <v>0.99729999999999996</v>
       </c>
       <c r="F53">
-        <v>0.95909999999999995</v>
+        <v>1.1705000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C54">
-        <v>0.58360000000000001</v>
+        <v>0.5696</v>
       </c>
       <c r="D54">
-        <v>0.54259999999999997</v>
+        <v>0.53900000000000003</v>
       </c>
       <c r="E54">
-        <v>0.7671</v>
+        <v>0.80110000000000003</v>
       </c>
       <c r="F54">
-        <v>0.92400000000000004</v>
+        <v>0.95909999999999995</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C55">
-        <v>0.59719999999999995</v>
+        <v>0.58360000000000001</v>
       </c>
       <c r="D55">
-        <v>0.55259999999999998</v>
+        <v>0.54259999999999997</v>
       </c>
       <c r="E55">
-        <v>0.77690000000000003</v>
+        <v>0.7671</v>
       </c>
       <c r="F55">
-        <v>0.93310000000000004</v>
+        <v>0.92400000000000004</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56">
+        <v>0.59719999999999995</v>
+      </c>
+      <c r="D56">
+        <v>0.55259999999999998</v>
+      </c>
+      <c r="E56">
+        <v>0.77690000000000003</v>
+      </c>
+      <c r="F56">
+        <v>0.93310000000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
         <v>32</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>0.63500000000000001</v>
       </c>
-      <c r="D56">
+      <c r="D57">
         <v>0.58089999999999997</v>
       </c>
-      <c r="E56">
+      <c r="E57">
         <v>0.7843</v>
       </c>
-      <c r="F56">
+      <c r="F57">
         <v>0.93359999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58">
+        <v>0.77180000000000004</v>
+      </c>
+      <c r="D58">
+        <v>0.8014</v>
+      </c>
+      <c r="E58">
+        <v>0.73829999999999996</v>
+      </c>
+      <c r="F58">
+        <v>0.85219999999999996</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="44" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="31" operator="greaterThan">
       <formula>$C$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3:C36">
-    <cfRule type="cellIs" dxfId="43" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="greaterThan">
       <formula>$C$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3:D36">
-    <cfRule type="cellIs" dxfId="42" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="28" operator="greaterThan">
+      <formula>$D$2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="29" operator="greaterThan">
       <formula>$D$1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="28" operator="greaterThan">
-      <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E36">
-    <cfRule type="cellIs" dxfId="40" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="27" operator="lessThan">
       <formula>$E$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F36">
-    <cfRule type="cellIs" dxfId="39" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="26" operator="lessThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39:C48">
-    <cfRule type="cellIs" dxfId="38" priority="25" operator="greaterThan">
+  <conditionalFormatting sqref="C39:C49">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="greaterThan">
       <formula>$C$38</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D39:D48">
-    <cfRule type="cellIs" dxfId="37" priority="23" operator="greaterThan">
+  <conditionalFormatting sqref="D39:D49">
+    <cfRule type="cellIs" dxfId="18" priority="23" operator="greaterThan">
       <formula>$D$38</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E39:E48">
-    <cfRule type="cellIs" dxfId="36" priority="22" operator="lessThan">
+  <conditionalFormatting sqref="E39:E49">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="lessThan">
       <formula>$E$38</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39:F48">
-    <cfRule type="cellIs" dxfId="35" priority="21" operator="lessThan">
+  <conditionalFormatting sqref="F39:F49">
+    <cfRule type="cellIs" dxfId="16" priority="21" operator="lessThan">
       <formula>$F$38</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51:C56">
-    <cfRule type="cellIs" dxfId="34" priority="20" operator="greaterThan">
-      <formula>$C$50</formula>
+  <conditionalFormatting sqref="C52:C58">
+    <cfRule type="top10" dxfId="15" priority="13" rank="1"/>
+    <cfRule type="cellIs" dxfId="14" priority="20" operator="greaterThan">
+      <formula>$C$51</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="33" priority="13" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D51:D56">
-    <cfRule type="cellIs" dxfId="32" priority="19" operator="greaterThan">
-      <formula>$D$50</formula>
+  <conditionalFormatting sqref="D52:D58">
+    <cfRule type="top10" dxfId="13" priority="12" rank="1"/>
+    <cfRule type="cellIs" dxfId="12" priority="19" operator="greaterThan">
+      <formula>$D$51</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="31" priority="12" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E51:E56">
-    <cfRule type="cellIs" dxfId="30" priority="18" operator="lessThan">
-      <formula>$E$50</formula>
+  <conditionalFormatting sqref="E52:E58">
+    <cfRule type="top10" dxfId="11" priority="10" bottom="1" rank="1"/>
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="lessThan">
+      <formula>$E$51</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="29" priority="10" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F51:F56">
-    <cfRule type="cellIs" dxfId="10" priority="17" operator="lessThan">
-      <formula>$F$50</formula>
+  <conditionalFormatting sqref="F52:F58">
+    <cfRule type="top10" dxfId="9" priority="9" bottom="1" rank="1"/>
+    <cfRule type="cellIs" dxfId="8" priority="17" operator="lessThan">
+      <formula>$F$51</formula>
     </cfRule>
-    <cfRule type="top10" dxfId="9" priority="9" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C48">
+  <conditionalFormatting sqref="C38:C49">
     <cfRule type="top10" dxfId="7" priority="8" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D38:D48">
+  <conditionalFormatting sqref="D38:D49">
     <cfRule type="top10" dxfId="6" priority="7" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E38:E48">
+  <conditionalFormatting sqref="E38:E49">
     <cfRule type="top10" dxfId="5" priority="6" bottom="1" rank="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38:F48">
+  <conditionalFormatting sqref="F38:F49">
     <cfRule type="top10" dxfId="4" priority="5" bottom="1" rank="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C36">

</xml_diff>